<commit_message>
Added Medium Viper animal companion.
Added Medium Viper animal companion.
</commit_message>
<xml_diff>
--- a/nwnds_notes/Animal Companions/AnimalCompanionWorksheet.xlsx
+++ b/nwnds_notes/Animal Companions/AnimalCompanionWorksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="315" windowWidth="27555" windowHeight="10785" tabRatio="843" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="600" yWindow="315" windowWidth="27555" windowHeight="10785" tabRatio="843" firstSheet="8" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Boneclaw_AC" sheetId="4" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="Z'tal_AC" sheetId="9" r:id="rId9"/>
     <sheet name="Kestrekel_AC" sheetId="10" r:id="rId10"/>
     <sheet name="Owl_AC" sheetId="11" r:id="rId11"/>
+    <sheet name="Viper, Medium_AC" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="106">
   <si>
     <t>Progression:</t>
   </si>
@@ -336,6 +337,12 @@
   </si>
   <si>
     <t>Alertness*</t>
+  </si>
+  <si>
+    <t>Improved Initiative*</t>
+  </si>
+  <si>
+    <t>Venom DC+</t>
   </si>
 </sst>
 </file>
@@ -2210,7 +2217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -2723,6 +2730,539 @@
         <v>23</v>
       </c>
       <c r="K22" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A4:K22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="4">
+        <v>2</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="2">
+        <f>SUM(G6+2)</f>
+        <v>4</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" ref="G8:G12" si="0">SUM(G7+2)</f>
+        <v>6</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="2">
+        <f>SUM(G12+2)</f>
+        <v>16</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" ref="G17:G22" si="1">SUM(G16+2)</f>
+        <v>18</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>